<commit_message>
solved errors in tests
</commit_message>
<xml_diff>
--- a/02_work_doc/01_daten/10_environmentalImpacts/Datenmodel_environmentalImpact.xlsx
+++ b/02_work_doc/01_daten/10_environmentalImpacts/Datenmodel_environmentalImpact.xlsx
@@ -40,6 +40,20 @@
 Ihre Version von Excel gestattet Ihnen das Lesen dieses Kommentarthreads. Jegliche Bearbeitungen daran werden jedoch entfernt, wenn die Datei in einer neueren Version von Excel geöffnet wird. Weitere Informationen: https://go.microsoft.com/fwlink/?linkid=870924.
 Kommentar:
     Kommt über EnArgus durch das FKZ. Hier nur zur Info.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="11"/>
+            <color rgb="FF000000"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Bitte hier den Namen des Bildes einfügen. Die Bilder bitte separat mitschicken.</t>
         </r>
       </text>
     </comment>
@@ -403,7 +417,7 @@
   <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="P21" activeCellId="0" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.73046875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -743,7 +757,7 @@
       <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="37.55"/>
   </cols>

</xml_diff>